<commit_message>
Revert "Ignore commit, only for accessing master"
This reverts commit 28de83f7f66bde21f9a4dc34c0a12e84ed052320.
</commit_message>
<xml_diff>
--- a/SetupSheets.xlsx
+++ b/SetupSheets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Journey\Documents\GitHub\LapSimCombined\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Code\LapSimCombined\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="540" windowWidth="9710" windowHeight="3240"/>
+    <workbookView xWindow="1815" yWindow="540" windowWidth="9705" windowHeight="3240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Combustion" sheetId="11" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="116">
   <si>
     <t>Date</t>
   </si>
@@ -368,9 +368,6 @@
   </si>
   <si>
     <t>Wf</t>
-  </si>
-  <si>
-    <t>CalPolySLO</t>
   </si>
 </sst>
 </file>
@@ -754,11 +751,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -813,7 +810,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -864,11 +861,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -974,11 +971,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1033,7 +1030,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1084,11 +1081,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1437,41 +1434,41 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:CV50"/>
+  <dimension ref="A1:CU50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="CQ6" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="BT6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CX10" sqref="CX9:CX10"/>
+      <selection pane="bottomRight" activeCell="CU6" sqref="CU6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="23" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="24" customWidth="1"/>
-    <col min="5" max="25" width="6.81640625" style="23" customWidth="1"/>
-    <col min="26" max="26" width="6.81640625" style="24" customWidth="1"/>
-    <col min="27" max="48" width="6.81640625" style="23" customWidth="1"/>
-    <col min="49" max="49" width="6.81640625" style="24" customWidth="1"/>
-    <col min="50" max="54" width="6.81640625" style="23" customWidth="1"/>
-    <col min="55" max="55" width="10.81640625" style="23" customWidth="1"/>
-    <col min="56" max="56" width="6.81640625" style="24" customWidth="1"/>
-    <col min="57" max="69" width="6.81640625" style="23" customWidth="1"/>
-    <col min="70" max="70" width="6.81640625" style="24" customWidth="1"/>
-    <col min="71" max="76" width="6.81640625" style="23" customWidth="1"/>
-    <col min="77" max="77" width="6.81640625" style="24" customWidth="1"/>
-    <col min="78" max="87" width="6.81640625" style="23" customWidth="1"/>
-    <col min="88" max="88" width="6.81640625" style="24" customWidth="1"/>
-    <col min="89" max="95" width="6.81640625" style="23" customWidth="1"/>
-    <col min="96" max="96" width="6.81640625" style="24" customWidth="1"/>
-    <col min="97" max="99" width="6.81640625" style="23" customWidth="1"/>
-    <col min="100" max="16384" width="9.1796875" style="23"/>
+    <col min="2" max="2" width="12.28515625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="24" customWidth="1"/>
+    <col min="5" max="25" width="6.85546875" style="23" customWidth="1"/>
+    <col min="26" max="26" width="6.85546875" style="24" customWidth="1"/>
+    <col min="27" max="48" width="6.85546875" style="23" customWidth="1"/>
+    <col min="49" max="49" width="6.85546875" style="24" customWidth="1"/>
+    <col min="50" max="54" width="6.85546875" style="23" customWidth="1"/>
+    <col min="55" max="55" width="10.85546875" style="23" customWidth="1"/>
+    <col min="56" max="56" width="6.85546875" style="24" customWidth="1"/>
+    <col min="57" max="69" width="6.85546875" style="23" customWidth="1"/>
+    <col min="70" max="70" width="6.85546875" style="24" customWidth="1"/>
+    <col min="71" max="76" width="6.85546875" style="23" customWidth="1"/>
+    <col min="77" max="77" width="6.85546875" style="24" customWidth="1"/>
+    <col min="78" max="87" width="6.85546875" style="23" customWidth="1"/>
+    <col min="88" max="88" width="6.85546875" style="24" customWidth="1"/>
+    <col min="89" max="95" width="6.85546875" style="23" customWidth="1"/>
+    <col min="96" max="96" width="6.85546875" style="24" customWidth="1"/>
+    <col min="97" max="99" width="6.85546875" style="23" customWidth="1"/>
+    <col min="100" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>35</v>
       </c>
@@ -1766,7 +1763,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:100" s="28" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="36"/>
       <c r="B2" s="26" t="s">
         <v>0</v>
@@ -2047,7 +2044,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:100" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
       <c r="B3" s="29"/>
       <c r="C3" s="30"/>
@@ -2148,7 +2145,7 @@
       <c r="CT3" s="15"/>
       <c r="CU3" s="15"/>
     </row>
-    <row r="4" spans="1:100" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="37"/>
       <c r="B4" s="29"/>
       <c r="C4" s="30"/>
@@ -2249,7 +2246,7 @@
       <c r="CT4" s="15"/>
       <c r="CU4" s="15"/>
     </row>
-    <row r="5" spans="1:100" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:99" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="51" t="s">
         <v>115</v>
       </c>
@@ -2604,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:100" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="49">
         <v>0</v>
       </c>
@@ -2886,11 +2883,8 @@
       <c r="CU6" s="45">
         <v>0</v>
       </c>
-      <c r="CV6" s="50" t="s">
-        <v>116</v>
-      </c>
     </row>
-    <row r="7" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A7" s="49">
         <v>1</v>
       </c>
@@ -3173,7 +3167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A8" s="49">
         <v>2</v>
       </c>
@@ -3456,7 +3450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A9" s="49"/>
       <c r="B9" s="48"/>
       <c r="C9" s="47"/>
@@ -3557,7 +3551,7 @@
       <c r="CT9" s="45"/>
       <c r="CU9" s="45"/>
     </row>
-    <row r="10" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A10" s="49"/>
       <c r="B10" s="48"/>
       <c r="C10" s="47"/>
@@ -3658,7 +3652,7 @@
       <c r="CT10" s="45"/>
       <c r="CU10" s="45"/>
     </row>
-    <row r="11" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A11" s="49"/>
       <c r="B11" s="48"/>
       <c r="C11" s="47"/>
@@ -3759,7 +3753,7 @@
       <c r="CT11" s="45"/>
       <c r="CU11" s="45"/>
     </row>
-    <row r="12" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A12" s="49"/>
       <c r="B12" s="48"/>
       <c r="C12" s="47"/>
@@ -3860,7 +3854,7 @@
       <c r="CT12" s="45"/>
       <c r="CU12" s="45"/>
     </row>
-    <row r="13" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A13" s="49"/>
       <c r="B13" s="48"/>
       <c r="C13" s="47"/>
@@ -3961,7 +3955,7 @@
       <c r="CT13" s="45"/>
       <c r="CU13" s="45"/>
     </row>
-    <row r="14" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A14" s="49"/>
       <c r="B14" s="48"/>
       <c r="C14" s="47"/>
@@ -4062,7 +4056,7 @@
       <c r="CT14" s="45"/>
       <c r="CU14" s="45"/>
     </row>
-    <row r="15" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A15" s="49"/>
       <c r="B15" s="48"/>
       <c r="C15" s="47"/>
@@ -4163,7 +4157,7 @@
       <c r="CT15" s="45"/>
       <c r="CU15" s="45"/>
     </row>
-    <row r="16" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A16" s="49"/>
       <c r="B16" s="48"/>
       <c r="C16" s="47"/>
@@ -4264,7 +4258,7 @@
       <c r="CT16" s="45"/>
       <c r="CU16" s="45"/>
     </row>
-    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A17" s="49"/>
       <c r="B17" s="48"/>
       <c r="C17" s="47"/>
@@ -4365,7 +4359,7 @@
       <c r="CT17" s="45"/>
       <c r="CU17" s="45"/>
     </row>
-    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A18" s="49"/>
       <c r="B18" s="48"/>
       <c r="C18" s="47"/>
@@ -4466,7 +4460,7 @@
       <c r="CT18" s="45"/>
       <c r="CU18" s="45"/>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A19" s="49"/>
       <c r="B19" s="48"/>
       <c r="C19" s="47"/>
@@ -4567,7 +4561,7 @@
       <c r="CT19" s="45"/>
       <c r="CU19" s="45"/>
     </row>
-    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A20" s="49"/>
       <c r="B20" s="48"/>
       <c r="C20" s="47"/>
@@ -4668,7 +4662,7 @@
       <c r="CT20" s="45"/>
       <c r="CU20" s="45"/>
     </row>
-    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A21" s="49"/>
       <c r="B21" s="48"/>
       <c r="C21" s="47"/>
@@ -4769,7 +4763,7 @@
       <c r="CT21" s="45"/>
       <c r="CU21" s="45"/>
     </row>
-    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A22" s="49"/>
       <c r="B22" s="48"/>
       <c r="C22" s="47"/>
@@ -4870,7 +4864,7 @@
       <c r="CT22" s="45"/>
       <c r="CU22" s="45"/>
     </row>
-    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A23" s="49"/>
       <c r="B23" s="48"/>
       <c r="C23" s="47"/>
@@ -4971,7 +4965,7 @@
       <c r="CT23" s="45"/>
       <c r="CU23" s="45"/>
     </row>
-    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A24" s="49"/>
       <c r="B24" s="48"/>
       <c r="C24" s="47"/>
@@ -5072,7 +5066,7 @@
       <c r="CT24" s="45"/>
       <c r="CU24" s="45"/>
     </row>
-    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A25" s="49"/>
       <c r="B25" s="48"/>
       <c r="C25" s="47"/>
@@ -5173,7 +5167,7 @@
       <c r="CT25" s="45"/>
       <c r="CU25" s="45"/>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A26" s="49"/>
       <c r="B26" s="48"/>
       <c r="C26" s="47"/>
@@ -5274,7 +5268,7 @@
       <c r="CT26" s="45"/>
       <c r="CU26" s="45"/>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A27" s="49"/>
       <c r="B27" s="48"/>
       <c r="C27" s="47"/>
@@ -5375,7 +5369,7 @@
       <c r="CT27" s="45"/>
       <c r="CU27" s="45"/>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A28" s="49"/>
       <c r="B28" s="48"/>
       <c r="C28" s="47"/>
@@ -5476,7 +5470,7 @@
       <c r="CT28" s="45"/>
       <c r="CU28" s="45"/>
     </row>
-    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A29" s="49"/>
       <c r="B29" s="48"/>
       <c r="C29" s="47"/>
@@ -5577,7 +5571,7 @@
       <c r="CT29" s="45"/>
       <c r="CU29" s="45"/>
     </row>
-    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A30" s="49"/>
       <c r="B30" s="48"/>
       <c r="C30" s="47"/>
@@ -5678,7 +5672,7 @@
       <c r="CT30" s="45"/>
       <c r="CU30" s="45"/>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A31" s="49"/>
       <c r="B31" s="48"/>
       <c r="C31" s="47"/>
@@ -5779,7 +5773,7 @@
       <c r="CT31" s="45"/>
       <c r="CU31" s="45"/>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A32" s="49"/>
       <c r="B32" s="48"/>
       <c r="C32" s="47"/>
@@ -5880,7 +5874,7 @@
       <c r="CT32" s="45"/>
       <c r="CU32" s="45"/>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A33" s="49"/>
       <c r="B33" s="48"/>
       <c r="C33" s="47"/>
@@ -5981,7 +5975,7 @@
       <c r="CT33" s="45"/>
       <c r="CU33" s="45"/>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A34" s="49"/>
       <c r="B34" s="48"/>
       <c r="C34" s="47"/>
@@ -6082,7 +6076,7 @@
       <c r="CT34" s="45"/>
       <c r="CU34" s="45"/>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A35" s="49"/>
       <c r="B35" s="48"/>
       <c r="C35" s="47"/>
@@ -6183,7 +6177,7 @@
       <c r="CT35" s="45"/>
       <c r="CU35" s="45"/>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A36" s="49"/>
       <c r="B36" s="48"/>
       <c r="C36" s="47"/>
@@ -6284,7 +6278,7 @@
       <c r="CT36" s="45"/>
       <c r="CU36" s="45"/>
     </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A37" s="49"/>
       <c r="B37" s="48"/>
       <c r="C37" s="47"/>
@@ -6385,7 +6379,7 @@
       <c r="CT37" s="45"/>
       <c r="CU37" s="45"/>
     </row>
-    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A38" s="49"/>
       <c r="B38" s="48"/>
       <c r="C38" s="47"/>
@@ -6486,7 +6480,7 @@
       <c r="CT38" s="45"/>
       <c r="CU38" s="45"/>
     </row>
-    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A39" s="49"/>
       <c r="B39" s="48"/>
       <c r="C39" s="47"/>
@@ -6587,7 +6581,7 @@
       <c r="CT39" s="45"/>
       <c r="CU39" s="45"/>
     </row>
-    <row r="40" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A40" s="49"/>
       <c r="B40" s="48"/>
       <c r="C40" s="47"/>
@@ -6688,7 +6682,7 @@
       <c r="CT40" s="45"/>
       <c r="CU40" s="45"/>
     </row>
-    <row r="41" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A41" s="49"/>
       <c r="B41" s="48"/>
       <c r="C41" s="47"/>
@@ -6789,7 +6783,7 @@
       <c r="CT41" s="45"/>
       <c r="CU41" s="45"/>
     </row>
-    <row r="42" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A42" s="49"/>
       <c r="B42" s="48"/>
       <c r="C42" s="47"/>
@@ -6890,7 +6884,7 @@
       <c r="CT42" s="45"/>
       <c r="CU42" s="45"/>
     </row>
-    <row r="43" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A43" s="49"/>
       <c r="B43" s="48"/>
       <c r="C43" s="47"/>
@@ -6991,31 +6985,31 @@
       <c r="CT43" s="45"/>
       <c r="CU43" s="45"/>
     </row>
-    <row r="44" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B44" s="31"/>
       <c r="C44" s="32"/>
     </row>
-    <row r="45" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B45" s="31"/>
       <c r="C45" s="32"/>
     </row>
-    <row r="46" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B46" s="31"/>
       <c r="C46" s="32"/>
     </row>
-    <row r="47" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B47" s="31"/>
       <c r="C47" s="32"/>
     </row>
-    <row r="48" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B48" s="31"/>
       <c r="C48" s="32"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="31"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="31"/>
       <c r="C50" s="32"/>
     </row>
@@ -7030,19 +7024,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>12700</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7050,7 +7044,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -7066,7 +7060,7 @@
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
@@ -7080,19 +7074,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>12700</xdr:rowOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7100,7 +7094,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7112,39 +7106,39 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:CU50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="23" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="24" customWidth="1"/>
-    <col min="5" max="25" width="6.81640625" style="23" customWidth="1"/>
-    <col min="26" max="26" width="6.81640625" style="24" customWidth="1"/>
-    <col min="27" max="48" width="6.81640625" style="23" customWidth="1"/>
-    <col min="49" max="49" width="6.81640625" style="24" customWidth="1"/>
-    <col min="50" max="54" width="6.81640625" style="23" customWidth="1"/>
-    <col min="55" max="55" width="10.81640625" style="23" customWidth="1"/>
-    <col min="56" max="56" width="6.81640625" style="24" customWidth="1"/>
-    <col min="57" max="69" width="6.81640625" style="23" customWidth="1"/>
-    <col min="70" max="70" width="6.81640625" style="24" customWidth="1"/>
-    <col min="71" max="76" width="6.81640625" style="23" customWidth="1"/>
-    <col min="77" max="77" width="6.81640625" style="24" customWidth="1"/>
-    <col min="78" max="87" width="6.81640625" style="23" customWidth="1"/>
-    <col min="88" max="88" width="6.81640625" style="24" customWidth="1"/>
-    <col min="89" max="95" width="6.81640625" style="23" customWidth="1"/>
-    <col min="96" max="96" width="6.81640625" style="24" customWidth="1"/>
-    <col min="97" max="99" width="6.81640625" style="23" customWidth="1"/>
-    <col min="100" max="16384" width="9.1796875" style="23"/>
+    <col min="2" max="2" width="12.28515625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="24" customWidth="1"/>
+    <col min="5" max="25" width="6.85546875" style="23" customWidth="1"/>
+    <col min="26" max="26" width="6.85546875" style="24" customWidth="1"/>
+    <col min="27" max="48" width="6.85546875" style="23" customWidth="1"/>
+    <col min="49" max="49" width="6.85546875" style="24" customWidth="1"/>
+    <col min="50" max="54" width="6.85546875" style="23" customWidth="1"/>
+    <col min="55" max="55" width="10.85546875" style="23" customWidth="1"/>
+    <col min="56" max="56" width="6.85546875" style="24" customWidth="1"/>
+    <col min="57" max="69" width="6.85546875" style="23" customWidth="1"/>
+    <col min="70" max="70" width="6.85546875" style="24" customWidth="1"/>
+    <col min="71" max="76" width="6.85546875" style="23" customWidth="1"/>
+    <col min="77" max="77" width="6.85546875" style="24" customWidth="1"/>
+    <col min="78" max="87" width="6.85546875" style="23" customWidth="1"/>
+    <col min="88" max="88" width="6.85546875" style="24" customWidth="1"/>
+    <col min="89" max="95" width="6.85546875" style="23" customWidth="1"/>
+    <col min="96" max="96" width="6.85546875" style="24" customWidth="1"/>
+    <col min="97" max="99" width="6.85546875" style="23" customWidth="1"/>
+    <col min="100" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>35</v>
       </c>
@@ -7439,7 +7433,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="36"/>
       <c r="B2" s="26" t="s">
         <v>0</v>
@@ -7720,7 +7714,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
       <c r="B3" s="29"/>
       <c r="C3" s="30"/>
@@ -7821,7 +7815,7 @@
       <c r="CT3" s="15"/>
       <c r="CU3" s="15"/>
     </row>
-    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="37"/>
       <c r="B4" s="29"/>
       <c r="C4" s="30"/>
@@ -7922,7 +7916,7 @@
       <c r="CT4" s="15"/>
       <c r="CU4" s="15"/>
     </row>
-    <row r="5" spans="1:99" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:99" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>36</v>
       </c>
@@ -8277,7 +8271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="1">
         <v>35065</v>
@@ -8560,7 +8554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
@@ -8661,7 +8655,7 @@
       <c r="CT7" s="18"/>
       <c r="CU7" s="18"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="1"/>
       <c r="C8" s="8"/>
@@ -8761,7 +8755,7 @@
       <c r="CT8" s="18"/>
       <c r="CU8" s="18"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="1"/>
       <c r="C9" s="8"/>
@@ -8862,7 +8856,7 @@
       <c r="CT9" s="18"/>
       <c r="CU9" s="18"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="1"/>
       <c r="C10" s="8"/>
@@ -8963,7 +8957,7 @@
       <c r="CT10" s="18"/>
       <c r="CU10" s="18"/>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="1"/>
       <c r="C11" s="8"/>
@@ -9064,7 +9058,7 @@
       <c r="CT11" s="18"/>
       <c r="CU11" s="18"/>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="1"/>
       <c r="C12" s="8"/>
@@ -9165,7 +9159,7 @@
       <c r="CT12" s="18"/>
       <c r="CU12" s="18"/>
     </row>
-    <row r="13" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="1"/>
       <c r="C13" s="8"/>
@@ -9266,7 +9260,7 @@
       <c r="CT13" s="18"/>
       <c r="CU13" s="18"/>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="1"/>
       <c r="C14" s="8"/>
@@ -9367,7 +9361,7 @@
       <c r="CT14" s="18"/>
       <c r="CU14" s="18"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8"/>
@@ -9468,7 +9462,7 @@
       <c r="CT15" s="18"/>
       <c r="CU15" s="18"/>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="1"/>
       <c r="C16" s="8"/>
@@ -9569,7 +9563,7 @@
       <c r="CT16" s="18"/>
       <c r="CU16" s="18"/>
     </row>
-    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8"/>
@@ -9670,7 +9664,7 @@
       <c r="CT17" s="18"/>
       <c r="CU17" s="18"/>
     </row>
-    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="1"/>
       <c r="C18" s="8"/>
@@ -9771,7 +9765,7 @@
       <c r="CT18" s="18"/>
       <c r="CU18" s="18"/>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" s="1"/>
       <c r="C19" s="8"/>
@@ -9872,7 +9866,7 @@
       <c r="CT19" s="18"/>
       <c r="CU19" s="18"/>
     </row>
-    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="1"/>
       <c r="C20" s="8"/>
@@ -9973,7 +9967,7 @@
       <c r="CT20" s="18"/>
       <c r="CU20" s="18"/>
     </row>
-    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" s="1"/>
       <c r="C21" s="8"/>
@@ -10074,7 +10068,7 @@
       <c r="CT21" s="18"/>
       <c r="CU21" s="18"/>
     </row>
-    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" s="1"/>
       <c r="C22" s="8"/>
@@ -10175,7 +10169,7 @@
       <c r="CT22" s="18"/>
       <c r="CU22" s="18"/>
     </row>
-    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
       <c r="B23" s="1"/>
       <c r="C23" s="8"/>
@@ -10276,7 +10270,7 @@
       <c r="CT23" s="18"/>
       <c r="CU23" s="18"/>
     </row>
-    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
       <c r="B24" s="1"/>
       <c r="C24" s="8"/>
@@ -10377,7 +10371,7 @@
       <c r="CT24" s="18"/>
       <c r="CU24" s="18"/>
     </row>
-    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" s="1"/>
       <c r="C25" s="8"/>
@@ -10478,7 +10472,7 @@
       <c r="CT25" s="18"/>
       <c r="CU25" s="18"/>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
       <c r="B26" s="1"/>
       <c r="C26" s="8"/>
@@ -10579,7 +10573,7 @@
       <c r="CT26" s="18"/>
       <c r="CU26" s="18"/>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" s="1"/>
       <c r="C27" s="8"/>
@@ -10680,7 +10674,7 @@
       <c r="CT27" s="18"/>
       <c r="CU27" s="18"/>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
       <c r="B28" s="1"/>
       <c r="C28" s="8"/>
@@ -10781,7 +10775,7 @@
       <c r="CT28" s="18"/>
       <c r="CU28" s="18"/>
     </row>
-    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
       <c r="B29" s="1"/>
       <c r="C29" s="8"/>
@@ -10882,87 +10876,87 @@
       <c r="CT29" s="18"/>
       <c r="CU29" s="18"/>
     </row>
-    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B31" s="31"/>
       <c r="C31" s="32"/>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:99" x14ac:dyDescent="0.2">
       <c r="B32" s="31"/>
       <c r="C32" s="32"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="31"/>
       <c r="C33" s="32"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="31"/>
       <c r="C34" s="32"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="31"/>
       <c r="C35" s="32"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" s="31"/>
       <c r="C36" s="32"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" s="31"/>
       <c r="C37" s="32"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" s="31"/>
       <c r="C38" s="32"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="31"/>
       <c r="C39" s="32"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" s="31"/>
       <c r="C40" s="32"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" s="31"/>
       <c r="C41" s="32"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" s="31"/>
       <c r="C42" s="32"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" s="31"/>
       <c r="C43" s="32"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" s="31"/>
       <c r="C44" s="32"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" s="31"/>
       <c r="C45" s="32"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B46" s="31"/>
       <c r="C46" s="32"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B47" s="31"/>
       <c r="C47" s="32"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" s="31"/>
       <c r="C48" s="32"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="31"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="31"/>
       <c r="C50" s="32"/>
     </row>
@@ -10977,19 +10971,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>12700</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -10997,7 +10991,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11013,7 +11007,7 @@
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
@@ -11027,19 +11021,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>12700</xdr:rowOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -11047,7 +11041,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Update setup sheet for predicated 2017 e-car parameters
</commit_message>
<xml_diff>
--- a/SetupSheets.xlsx
+++ b/SetupSheets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Code\LapSimCombined\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Combustion" sheetId="11" r:id="rId1"/>
     <sheet name="Electric" sheetId="8" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" refMode="R1C1"/>
+  <calcPr calcId="171027" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -373,7 +373,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-C09]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -1246,6 +1246,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1281,6 +1298,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7024,19 +7058,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7044,7 +7078,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -7074,19 +7108,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7094,7 +7128,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7107,10 +7141,10 @@
   <dimension ref="A1:CU50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="BZ6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Y6" sqref="Y6"/>
+      <selection pane="bottomRight" activeCell="CR6" sqref="CR6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8283,7 +8317,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="18">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F6" s="18">
         <v>48</v>
@@ -8322,19 +8356,19 @@
         <v>0</v>
       </c>
       <c r="R6" s="18">
-        <v>34.200000000000003</v>
+        <v>31.72</v>
       </c>
       <c r="S6" s="18">
         <v>0</v>
       </c>
       <c r="T6" s="41">
-        <v>10.25</v>
+        <v>9</v>
       </c>
       <c r="U6" s="18">
         <v>0</v>
       </c>
       <c r="V6" s="18">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="W6" s="18">
         <v>0</v>
@@ -8343,7 +8377,7 @@
         <v>9.5</v>
       </c>
       <c r="Y6" s="12">
-        <v>604</v>
+        <v>615</v>
       </c>
       <c r="Z6" s="17"/>
       <c r="AA6" s="18">
@@ -8436,7 +8470,7 @@
         <v>1</v>
       </c>
       <c r="BF6" s="12">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="BG6" s="12">
         <v>0</v>
@@ -8501,10 +8535,10 @@
         <v>0</v>
       </c>
       <c r="CC6" s="12">
-        <v>0.45</v>
+        <v>0.7</v>
       </c>
       <c r="CD6" s="12">
-        <v>-0.89</v>
+        <v>-1.2</v>
       </c>
       <c r="CE6" s="12">
         <v>2015</v>
@@ -8513,7 +8547,7 @@
         <v>2.3289999999999999E-3</v>
       </c>
       <c r="CG6" s="12">
-        <v>34.25</v>
+        <v>31.72</v>
       </c>
       <c r="CH6" s="12">
         <v>0</v>
@@ -10971,19 +11005,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -10991,7 +11025,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11021,19 +11055,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -11041,7 +11075,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Resolve Mass/Weight related errors.
* No longer uses mass pretty much anywhere.
   * Everywhere it said mass, it pretty much meant weight. Some parts of the code had treated lbs as slugs as a result.
* Simplifies handling of mass properties.
   * It's now only necessary to fill in car weight & CG, driver weight & CG, and unsprung weight information.
* Eliminates CarChassis class that was never clearly delineated in purpose from Car.
* Add a grip scaling factor to the CarTire to allow easy scaling of the Tire Model to give more realistic grip levels.
* Update SetupSheets with correct mass information.
</commit_message>
<xml_diff>
--- a/SetupSheets.xlsx
+++ b/SetupSheets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Code\LapSimCombined\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -7058,19 +7058,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7078,7 +7078,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -7108,19 +7108,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7128,7 +7128,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7141,10 +7141,10 @@
   <dimension ref="A1:CU50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BZ6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CR6" sqref="CR6"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8320,10 +8320,10 @@
         <v>61</v>
       </c>
       <c r="F6" s="18">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="18">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H6" s="18">
         <v>0</v>
@@ -8365,10 +8365,10 @@
         <v>9</v>
       </c>
       <c r="U6" s="18">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="V6" s="18">
-        <v>30</v>
+        <v>31.72</v>
       </c>
       <c r="W6" s="18">
         <v>0</v>
@@ -8377,7 +8377,7 @@
         <v>9.5</v>
       </c>
       <c r="Y6" s="12">
-        <v>615</v>
+        <v>475</v>
       </c>
       <c r="Z6" s="17"/>
       <c r="AA6" s="18">
@@ -8399,10 +8399,10 @@
         <v>0</v>
       </c>
       <c r="AG6" s="18">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="AH6" s="18">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="AI6" s="18">
         <v>10.25</v>
@@ -8557,7 +8557,7 @@
       </c>
       <c r="CJ6" s="17"/>
       <c r="CK6" s="18">
-        <v>4.7</v>
+        <v>6.5</v>
       </c>
       <c r="CL6" s="18">
         <v>0</v>
@@ -11005,19 +11005,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -11025,7 +11025,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11055,19 +11055,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -11075,7 +11075,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Update unsprung weight naming in SetupSheets.
</commit_message>
<xml_diff>
--- a/SetupSheets.xlsx
+++ b/SetupSheets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="540" windowWidth="9705" windowHeight="3240" activeTab="1"/>
+    <workbookView xWindow="1815" yWindow="540" windowWidth="9705" windowHeight="3240"/>
   </bookViews>
   <sheets>
     <sheet name="Combustion" sheetId="11" r:id="rId1"/>
@@ -244,12 +244,6 @@
     <t>Spring Rate Rear</t>
   </si>
   <si>
-    <t>Unsprung Mass Front</t>
-  </si>
-  <si>
-    <t>Unsprung Mass Rear</t>
-  </si>
-  <si>
     <t>Pitch Center Front</t>
   </si>
   <si>
@@ -368,6 +362,12 @@
   </si>
   <si>
     <t>Wf</t>
+  </si>
+  <si>
+    <t>Unsprung Weight Front</t>
+  </si>
+  <si>
+    <t>Unsprung Weight Rear</t>
   </si>
 </sst>
 </file>
@@ -1470,11 +1470,11 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:CU50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BT6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="X6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CU6" sqref="CU6"/>
+      <selection pane="bottomRight" activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1509,7 +1509,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="7"/>
       <c r="D1" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -1593,13 +1593,13 @@
         <v>43</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="AI1" s="2" t="s">
         <v>66</v>
@@ -1614,7 +1614,7 @@
         <v>17</v>
       </c>
       <c r="AM1" s="38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AN1" s="38" t="s">
         <v>18</v>
@@ -1632,16 +1632,16 @@
         <v>22</v>
       </c>
       <c r="AS1" s="38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AT1" s="38" t="s">
         <v>23</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AV1" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AW1" s="3" t="s">
         <v>45</v>
@@ -1662,7 +1662,7 @@
         <v>50</v>
       </c>
       <c r="BC1" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="BD1" s="3" t="s">
         <v>24</v>
@@ -1671,7 +1671,7 @@
         <v>25</v>
       </c>
       <c r="BF1" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="BG1" s="2" t="s">
         <v>26</v>
@@ -1686,22 +1686,22 @@
         <v>29</v>
       </c>
       <c r="BK1" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="BL1" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="BM1" s="2" t="s">
         <v>51</v>
       </c>
       <c r="BN1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="BP1" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="BO1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="BP1" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="BQ1" s="2" t="s">
         <v>49</v>
@@ -1719,10 +1719,10 @@
         <v>43</v>
       </c>
       <c r="BV1" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="BW1" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="BX1" s="2" t="s">
         <v>49</v>
@@ -1743,58 +1743,58 @@
         <v>53</v>
       </c>
       <c r="CD1" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="CE1" s="2" t="s">
         <v>54</v>
       </c>
       <c r="CF1" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="CG1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="CI1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="CH1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="CI1" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="CJ1" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="CK1" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="CL1" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="CM1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="CN1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="CO1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="CN1" s="6" t="s">
+      <c r="CP1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="CO1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="CP1" s="6" t="s">
+      <c r="CQ1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="CS1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="CT1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="CQ1" s="6" t="s">
+      <c r="CU1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="CR1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="CS1" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="CT1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="CU1" s="6" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:99" s="28" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -1953,7 +1953,7 @@
         <v>38</v>
       </c>
       <c r="BC2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="BD2" s="9"/>
       <c r="BE2" s="39" t="s">
@@ -2034,7 +2034,7 @@
         <v>59</v>
       </c>
       <c r="CF2" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="CG2" s="44" t="s">
         <v>37</v>
@@ -2047,35 +2047,35 @@
       </c>
       <c r="CJ2" s="9"/>
       <c r="CK2" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="CL2" s="11" t="s">
         <v>38</v>
       </c>
       <c r="CM2" s="42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="CN2" s="42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="CO2" s="42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="CP2" s="42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="CQ2" s="42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="CR2" s="9"/>
       <c r="CS2" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="CT2" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="CU2" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2282,7 +2282,7 @@
     </row>
     <row r="5" spans="1:99" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="51" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="30"/>
@@ -7140,11 +7140,11 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:CU50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="AF14" sqref="AF14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7179,7 +7179,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="7"/>
       <c r="D1" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -7263,13 +7263,13 @@
         <v>43</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="AI1" s="2" t="s">
         <v>66</v>
@@ -7284,7 +7284,7 @@
         <v>17</v>
       </c>
       <c r="AM1" s="38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AN1" s="38" t="s">
         <v>18</v>
@@ -7302,16 +7302,16 @@
         <v>22</v>
       </c>
       <c r="AS1" s="38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AT1" s="38" t="s">
         <v>23</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AV1" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AW1" s="3" t="s">
         <v>45</v>
@@ -7332,7 +7332,7 @@
         <v>50</v>
       </c>
       <c r="BC1" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="BD1" s="3" t="s">
         <v>24</v>
@@ -7341,7 +7341,7 @@
         <v>25</v>
       </c>
       <c r="BF1" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="BG1" s="2" t="s">
         <v>26</v>
@@ -7356,22 +7356,22 @@
         <v>29</v>
       </c>
       <c r="BK1" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="BL1" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="BM1" s="2" t="s">
         <v>51</v>
       </c>
       <c r="BN1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="BP1" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="BO1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="BP1" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="BQ1" s="2" t="s">
         <v>49</v>
@@ -7389,10 +7389,10 @@
         <v>43</v>
       </c>
       <c r="BV1" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="BW1" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="BX1" s="2" t="s">
         <v>49</v>
@@ -7413,58 +7413,58 @@
         <v>53</v>
       </c>
       <c r="CD1" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="CE1" s="2" t="s">
         <v>54</v>
       </c>
       <c r="CF1" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="CG1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="CI1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="CH1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="CI1" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="CJ1" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="CK1" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="CL1" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="CM1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="CN1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="CO1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="CN1" s="6" t="s">
+      <c r="CP1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="CO1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="CP1" s="6" t="s">
+      <c r="CQ1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="CS1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="CT1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="CQ1" s="6" t="s">
+      <c r="CU1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="CR1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="CS1" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="CT1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="CU1" s="6" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:99" s="28" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -7623,7 +7623,7 @@
         <v>38</v>
       </c>
       <c r="BC2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="BD2" s="9"/>
       <c r="BE2" s="39" t="s">
@@ -7704,7 +7704,7 @@
         <v>59</v>
       </c>
       <c r="CF2" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="CG2" s="44" t="s">
         <v>37</v>
@@ -7717,35 +7717,35 @@
       </c>
       <c r="CJ2" s="9"/>
       <c r="CK2" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="CL2" s="11" t="s">
         <v>38</v>
       </c>
       <c r="CM2" s="42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="CN2" s="42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="CO2" s="42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="CP2" s="42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="CQ2" s="42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="CR2" s="9"/>
       <c r="CS2" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="CT2" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="CU2" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8463,7 +8463,7 @@
         <v>70.396699999999996</v>
       </c>
       <c r="BC6" s="40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="BD6" s="17"/>
       <c r="BE6" s="12">

</xml_diff>